<commit_message>
combined add data into one spreadsheet
</commit_message>
<xml_diff>
--- a/private/colleen/results/resultsColleen/organizationOfData.xlsx
+++ b/private/colleen/results/resultsColleen/organizationOfData.xlsx
@@ -14,6 +14,7 @@
     <sheet name="BB ML 12_1_14" sheetId="6" r:id="rId9"/>
     <sheet name="DB ML 12_2_14" sheetId="7" r:id="rId10"/>
     <sheet name="BB MR 12_3 Various Tau" sheetId="8" r:id="rId11"/>
+    <sheet name="All Stimulus Types 12_4_14" sheetId="9" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
@@ -308,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -751,13 +752,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1116,6 +1132,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11101,4 +11138,2373 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:N58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="120" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="120" customWidth="1"/>
+    <col min="3" max="3" width="3.86719" style="120" customWidth="1"/>
+    <col min="4" max="4" width="5.17969" style="120" customWidth="1"/>
+    <col min="5" max="5" width="5.05469" style="120" customWidth="1"/>
+    <col min="6" max="6" width="4.17969" style="120" customWidth="1"/>
+    <col min="7" max="7" width="7.92969" style="120" customWidth="1"/>
+    <col min="8" max="8" width="5.67969" style="120" customWidth="1"/>
+    <col min="9" max="9" width="8.55469" style="120" customWidth="1"/>
+    <col min="10" max="10" width="5.67969" style="120" customWidth="1"/>
+    <col min="11" max="11" width="7.42969" style="120" customWidth="1"/>
+    <col min="12" max="12" width="5.67969" style="120" customWidth="1"/>
+    <col min="13" max="13" width="8.05469" style="120" customWidth="1"/>
+    <col min="14" max="14" width="7.58594" style="120" customWidth="1"/>
+    <col min="15" max="256" width="12.25" style="120" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.15" customHeight="1">
+      <c r="B2" t="s" s="79">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="65">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s" s="65">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s" s="65">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s" s="65">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s" s="65">
+        <v>6</v>
+      </c>
+      <c r="H2" s="65"/>
+      <c r="I2" t="s" s="65">
+        <v>7</v>
+      </c>
+      <c r="J2" s="65"/>
+      <c r="K2" t="s" s="65">
+        <v>8</v>
+      </c>
+      <c r="L2" s="119"/>
+      <c r="M2" t="s" s="65">
+        <v>9</v>
+      </c>
+      <c r="N2" s="119"/>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="B3" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C3" s="68">
+        <v>10</v>
+      </c>
+      <c r="D3" s="68">
+        <v>2</v>
+      </c>
+      <c r="E3" s="68">
+        <v>4</v>
+      </c>
+      <c r="F3" s="68">
+        <v>8</v>
+      </c>
+      <c r="G3" s="68">
+        <v>48.2458</v>
+      </c>
+      <c r="H3" s="68">
+        <v>0.4746</v>
+      </c>
+      <c r="I3" s="68">
+        <v>48.2118</v>
+      </c>
+      <c r="J3" s="68">
+        <v>0.3992</v>
+      </c>
+      <c r="K3" s="68">
+        <v>48.2525</v>
+      </c>
+      <c r="L3" s="68">
+        <v>0.8105</v>
+      </c>
+      <c r="M3" s="68">
+        <v>0</v>
+      </c>
+      <c r="N3" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="B4" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C4" s="72">
+        <v>11</v>
+      </c>
+      <c r="D4" s="72">
+        <v>1</v>
+      </c>
+      <c r="E4" s="72">
+        <v>4</v>
+      </c>
+      <c r="F4" s="72">
+        <v>16</v>
+      </c>
+      <c r="G4" s="72">
+        <v>48.1782</v>
+      </c>
+      <c r="H4" s="72">
+        <v>0.6345</v>
+      </c>
+      <c r="I4" s="72">
+        <v>48.2217</v>
+      </c>
+      <c r="J4" s="72">
+        <v>0.3242</v>
+      </c>
+      <c r="K4" s="72">
+        <v>48.6505</v>
+      </c>
+      <c r="L4" s="72">
+        <v>1.2637</v>
+      </c>
+      <c r="M4" s="72">
+        <v>0</v>
+      </c>
+      <c r="N4" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="B5" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C5" s="68">
+        <v>2</v>
+      </c>
+      <c r="D5" s="68">
+        <v>9</v>
+      </c>
+      <c r="E5" s="68">
+        <v>8</v>
+      </c>
+      <c r="F5" s="68">
+        <v>8</v>
+      </c>
+      <c r="G5" s="68">
+        <v>96.2906</v>
+      </c>
+      <c r="H5" s="68">
+        <v>0.7759</v>
+      </c>
+      <c r="I5" s="68">
+        <v>97.0162</v>
+      </c>
+      <c r="J5" s="68">
+        <v>1.1235</v>
+      </c>
+      <c r="K5" s="68">
+        <v>96.008</v>
+      </c>
+      <c r="L5" s="68">
+        <v>1.4017</v>
+      </c>
+      <c r="M5" s="68">
+        <v>0</v>
+      </c>
+      <c r="N5" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="B6" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C6" s="72">
+        <v>6</v>
+      </c>
+      <c r="D6" s="72">
+        <v>3</v>
+      </c>
+      <c r="E6" s="72">
+        <v>8</v>
+      </c>
+      <c r="F6" s="72">
+        <v>8</v>
+      </c>
+      <c r="G6" s="72">
+        <v>96.37779999999999</v>
+      </c>
+      <c r="H6" s="72">
+        <v>0.8529</v>
+      </c>
+      <c r="I6" s="72">
+        <v>96.68340000000001</v>
+      </c>
+      <c r="J6" s="72">
+        <v>1.625</v>
+      </c>
+      <c r="K6" s="72">
+        <v>95.8793</v>
+      </c>
+      <c r="L6" s="72">
+        <v>1.7374</v>
+      </c>
+      <c r="M6" s="72">
+        <v>0</v>
+      </c>
+      <c r="N6" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="B7" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C7" s="68">
+        <v>12</v>
+      </c>
+      <c r="D7" s="68">
+        <v>14</v>
+      </c>
+      <c r="E7" s="68">
+        <v>8</v>
+      </c>
+      <c r="F7" s="68">
+        <v>8</v>
+      </c>
+      <c r="G7" s="68">
+        <v>94.2439</v>
+      </c>
+      <c r="H7" s="68">
+        <v>1.4895</v>
+      </c>
+      <c r="I7" s="68">
+        <v>92.6371</v>
+      </c>
+      <c r="J7" s="68">
+        <v>1.6115</v>
+      </c>
+      <c r="K7" s="68">
+        <v>95.72920000000001</v>
+      </c>
+      <c r="L7" s="68">
+        <v>1.5379</v>
+      </c>
+      <c r="M7" s="68">
+        <v>103.0478</v>
+      </c>
+      <c r="N7" s="68">
+        <v>26.2789</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="B8" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C8" s="72">
+        <v>15</v>
+      </c>
+      <c r="D8" s="72">
+        <v>3</v>
+      </c>
+      <c r="E8" s="72">
+        <v>8</v>
+      </c>
+      <c r="F8" s="72">
+        <v>8</v>
+      </c>
+      <c r="G8" s="72">
+        <v>93.36369999999999</v>
+      </c>
+      <c r="H8" s="72">
+        <v>1.6917</v>
+      </c>
+      <c r="I8" s="72">
+        <v>92.80200000000001</v>
+      </c>
+      <c r="J8" s="72">
+        <v>1.8534</v>
+      </c>
+      <c r="K8" s="72">
+        <v>95.16670000000001</v>
+      </c>
+      <c r="L8" s="72">
+        <v>1.6961</v>
+      </c>
+      <c r="M8" s="72">
+        <v>91.1863</v>
+      </c>
+      <c r="N8" s="72">
+        <v>12.34785</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="B9" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C9" s="68">
+        <v>7</v>
+      </c>
+      <c r="D9" s="68">
+        <v>3</v>
+      </c>
+      <c r="E9" s="68">
+        <v>8</v>
+      </c>
+      <c r="F9" s="68">
+        <v>16</v>
+      </c>
+      <c r="G9" s="68">
+        <v>96.2764</v>
+      </c>
+      <c r="H9" s="68">
+        <v>0.837</v>
+      </c>
+      <c r="I9" s="68">
+        <v>96.8241</v>
+      </c>
+      <c r="J9" s="68">
+        <v>1.0359</v>
+      </c>
+      <c r="K9" s="68">
+        <v>96.0624</v>
+      </c>
+      <c r="L9" s="68">
+        <v>1.9367</v>
+      </c>
+      <c r="M9" s="68">
+        <v>0</v>
+      </c>
+      <c r="N9" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="B10" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C10" s="72">
+        <v>18</v>
+      </c>
+      <c r="D10" s="72">
+        <v>1</v>
+      </c>
+      <c r="E10" s="72">
+        <v>8</v>
+      </c>
+      <c r="F10" s="72">
+        <v>16</v>
+      </c>
+      <c r="G10" s="72">
+        <v>93.47450000000001</v>
+      </c>
+      <c r="H10" s="72">
+        <v>1.4377</v>
+      </c>
+      <c r="I10" s="72">
+        <v>90.9224</v>
+      </c>
+      <c r="J10" s="72">
+        <v>1.4474</v>
+      </c>
+      <c r="K10" s="72">
+        <v>93.51130000000001</v>
+      </c>
+      <c r="L10" s="72">
+        <v>1.7181</v>
+      </c>
+      <c r="M10" s="72">
+        <v>91.21339999999999</v>
+      </c>
+      <c r="N10" s="72">
+        <v>9.8567</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="B11" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C11" s="68">
+        <v>4</v>
+      </c>
+      <c r="D11" s="68">
+        <v>1</v>
+      </c>
+      <c r="E11" s="68">
+        <v>16</v>
+      </c>
+      <c r="F11" s="68">
+        <v>8</v>
+      </c>
+      <c r="G11" s="68">
+        <v>192.5311</v>
+      </c>
+      <c r="H11" s="68">
+        <v>5.2138</v>
+      </c>
+      <c r="I11" s="68">
+        <v>205.3461</v>
+      </c>
+      <c r="J11" s="68">
+        <v>19.8409</v>
+      </c>
+      <c r="K11" s="68">
+        <v>190.0693</v>
+      </c>
+      <c r="L11" s="68">
+        <v>16.9549</v>
+      </c>
+      <c r="M11" s="68">
+        <v>0</v>
+      </c>
+      <c r="N11" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="B12" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C12" s="72">
+        <v>16</v>
+      </c>
+      <c r="D12" s="72">
+        <v>4</v>
+      </c>
+      <c r="E12" s="72">
+        <v>16</v>
+      </c>
+      <c r="F12" s="72">
+        <v>8</v>
+      </c>
+      <c r="G12" s="72">
+        <v>184.6126</v>
+      </c>
+      <c r="H12" s="72">
+        <v>10.2005</v>
+      </c>
+      <c r="I12" s="72">
+        <v>176.4689</v>
+      </c>
+      <c r="J12" s="72">
+        <v>16.2248</v>
+      </c>
+      <c r="K12" s="72">
+        <v>190.8418</v>
+      </c>
+      <c r="L12" s="72">
+        <v>24.8675</v>
+      </c>
+      <c r="M12" s="72">
+        <v>194.7933</v>
+      </c>
+      <c r="N12" s="72">
+        <v>101.331</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="B13" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C13" s="68">
+        <v>5</v>
+      </c>
+      <c r="D13" s="68">
+        <v>4</v>
+      </c>
+      <c r="E13" s="68">
+        <v>16</v>
+      </c>
+      <c r="F13" s="68">
+        <v>16</v>
+      </c>
+      <c r="G13" s="68">
+        <v>192.3259</v>
+      </c>
+      <c r="H13" s="68">
+        <v>3.5522</v>
+      </c>
+      <c r="I13" s="68">
+        <v>195.878</v>
+      </c>
+      <c r="J13" s="68">
+        <v>5.8959</v>
+      </c>
+      <c r="K13" s="68">
+        <v>188.395</v>
+      </c>
+      <c r="L13" s="68">
+        <v>7.8328</v>
+      </c>
+      <c r="M13" s="68">
+        <v>0</v>
+      </c>
+      <c r="N13" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="B14" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C14" s="72">
+        <v>3</v>
+      </c>
+      <c r="D14" s="72">
+        <v>23</v>
+      </c>
+      <c r="E14" s="72">
+        <v>16</v>
+      </c>
+      <c r="F14" s="72">
+        <v>16</v>
+      </c>
+      <c r="G14" s="72">
+        <v>191.386</v>
+      </c>
+      <c r="H14" s="72">
+        <v>2.8556</v>
+      </c>
+      <c r="I14" s="72">
+        <v>195.3012</v>
+      </c>
+      <c r="J14" s="72">
+        <v>5.5379</v>
+      </c>
+      <c r="K14" s="72">
+        <v>189.7446</v>
+      </c>
+      <c r="L14" s="72">
+        <v>6.1453</v>
+      </c>
+      <c r="M14" s="72">
+        <v>0</v>
+      </c>
+      <c r="N14" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="B15" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>13</v>
+      </c>
+      <c r="D15" s="68">
+        <v>1</v>
+      </c>
+      <c r="E15" s="68">
+        <v>16</v>
+      </c>
+      <c r="F15" s="68">
+        <v>16</v>
+      </c>
+      <c r="G15" s="68">
+        <v>187.57</v>
+      </c>
+      <c r="H15" s="68">
+        <v>4.4339</v>
+      </c>
+      <c r="I15" s="68">
+        <v>179.5899</v>
+      </c>
+      <c r="J15" s="68">
+        <v>6.3662</v>
+      </c>
+      <c r="K15" s="68">
+        <v>186.8455</v>
+      </c>
+      <c r="L15" s="68">
+        <v>6.7636</v>
+      </c>
+      <c r="M15" s="68">
+        <v>204.2783</v>
+      </c>
+      <c r="N15" s="68">
+        <v>82.68600000000001</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="B16" t="s" s="71">
+        <v>1</v>
+      </c>
+      <c r="C16" s="72">
+        <v>19</v>
+      </c>
+      <c r="D16" s="72">
+        <v>1</v>
+      </c>
+      <c r="E16" s="72">
+        <v>16</v>
+      </c>
+      <c r="F16" s="72">
+        <v>16</v>
+      </c>
+      <c r="G16" s="72">
+        <v>183.9616</v>
+      </c>
+      <c r="H16" s="72">
+        <v>4.7369</v>
+      </c>
+      <c r="I16" s="72">
+        <v>177.588</v>
+      </c>
+      <c r="J16" s="72">
+        <v>9.0639</v>
+      </c>
+      <c r="K16" s="72">
+        <v>187.5362</v>
+      </c>
+      <c r="L16" s="72">
+        <v>12.5737</v>
+      </c>
+      <c r="M16" s="72">
+        <v>199.0751</v>
+      </c>
+      <c r="N16" s="72">
+        <v>75.28319999999999</v>
+      </c>
+    </row>
+    <row r="17" ht="20.15" customHeight="1">
+      <c r="B17" t="s" s="85">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s" s="68">
+        <v>18</v>
+      </c>
+      <c r="D17" s="89">
+        <v>2</v>
+      </c>
+      <c r="E17" s="90">
+        <v>8</v>
+      </c>
+      <c r="F17" s="68">
+        <v>8</v>
+      </c>
+      <c r="G17" s="68">
+        <v>93.1327</v>
+      </c>
+      <c r="H17" s="68">
+        <v>2.5905</v>
+      </c>
+      <c r="I17" s="68">
+        <v>93.9007</v>
+      </c>
+      <c r="J17" s="68">
+        <v>0.7951</v>
+      </c>
+      <c r="K17" s="68">
+        <v>94.3198</v>
+      </c>
+      <c r="L17" s="68">
+        <v>1.3409</v>
+      </c>
+      <c r="M17" s="68">
+        <v>96.5501</v>
+      </c>
+      <c r="N17" s="68">
+        <v>19.6723</v>
+      </c>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="B18" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s" s="72">
+        <v>19</v>
+      </c>
+      <c r="D18" s="86">
+        <v>4</v>
+      </c>
+      <c r="E18" s="87">
+        <v>8</v>
+      </c>
+      <c r="F18" s="72">
+        <v>8</v>
+      </c>
+      <c r="G18" s="72">
+        <v>90.82429999999999</v>
+      </c>
+      <c r="H18" s="72">
+        <v>3.2959</v>
+      </c>
+      <c r="I18" s="72">
+        <v>92.75</v>
+      </c>
+      <c r="J18" s="72">
+        <v>0.7907</v>
+      </c>
+      <c r="K18" s="72">
+        <v>93.8439</v>
+      </c>
+      <c r="L18" s="72">
+        <v>2.1854</v>
+      </c>
+      <c r="M18" s="72">
+        <v>90.4033</v>
+      </c>
+      <c r="N18" s="72">
+        <v>27.6925</v>
+      </c>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="B19" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s" s="68">
+        <v>20</v>
+      </c>
+      <c r="D19" s="89">
+        <v>4</v>
+      </c>
+      <c r="E19" s="90">
+        <v>8</v>
+      </c>
+      <c r="F19" s="68">
+        <v>16</v>
+      </c>
+      <c r="G19" s="68">
+        <v>91.01349999999999</v>
+      </c>
+      <c r="H19" s="68">
+        <v>2.6286</v>
+      </c>
+      <c r="I19" s="68">
+        <v>92.2978</v>
+      </c>
+      <c r="J19" s="68">
+        <v>0.6092</v>
+      </c>
+      <c r="K19" s="68">
+        <v>91.9926</v>
+      </c>
+      <c r="L19" s="68">
+        <v>2.5153</v>
+      </c>
+      <c r="M19" s="68">
+        <v>93.3387</v>
+      </c>
+      <c r="N19" s="68">
+        <v>8.917</v>
+      </c>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="B20" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="72">
+        <v>21</v>
+      </c>
+      <c r="D20" s="86">
+        <v>1</v>
+      </c>
+      <c r="E20" s="87">
+        <v>16</v>
+      </c>
+      <c r="F20" s="72">
+        <v>8</v>
+      </c>
+      <c r="G20" s="72">
+        <v>184.1164</v>
+      </c>
+      <c r="H20" s="72">
+        <v>24.505</v>
+      </c>
+      <c r="I20" s="72">
+        <v>182.9856</v>
+      </c>
+      <c r="J20" s="72">
+        <v>5.3567</v>
+      </c>
+      <c r="K20" s="72">
+        <v>192.1703</v>
+      </c>
+      <c r="L20" s="72">
+        <v>24.8277</v>
+      </c>
+      <c r="M20" s="72">
+        <v>196.1818</v>
+      </c>
+      <c r="N20" s="72">
+        <v>50.5889</v>
+      </c>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="B21" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s" s="68">
+        <v>23</v>
+      </c>
+      <c r="D21" s="89">
+        <v>2</v>
+      </c>
+      <c r="E21" s="90">
+        <v>16</v>
+      </c>
+      <c r="F21" s="68">
+        <v>16</v>
+      </c>
+      <c r="G21" s="68">
+        <v>181.624</v>
+      </c>
+      <c r="H21" s="68">
+        <v>7.7479</v>
+      </c>
+      <c r="I21" s="68">
+        <v>183.4271</v>
+      </c>
+      <c r="J21" s="68">
+        <v>3.5344</v>
+      </c>
+      <c r="K21" s="68">
+        <v>183.6619</v>
+      </c>
+      <c r="L21" s="68">
+        <v>10.6257</v>
+      </c>
+      <c r="M21" s="68">
+        <v>188.1424</v>
+      </c>
+      <c r="N21" s="68">
+        <v>42.866</v>
+      </c>
+    </row>
+    <row r="22" ht="20.15" customHeight="1">
+      <c r="B22" t="s" s="91">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s" s="72">
+        <v>24</v>
+      </c>
+      <c r="D22" s="86">
+        <v>4</v>
+      </c>
+      <c r="E22" s="87">
+        <v>16</v>
+      </c>
+      <c r="F22" s="72">
+        <v>16</v>
+      </c>
+      <c r="G22" s="72">
+        <v>179.9152</v>
+      </c>
+      <c r="H22" s="72">
+        <v>10.0789</v>
+      </c>
+      <c r="I22" s="72">
+        <v>181.9082</v>
+      </c>
+      <c r="J22" s="72">
+        <v>5.0169</v>
+      </c>
+      <c r="K22" s="72">
+        <v>181.3347</v>
+      </c>
+      <c r="L22" s="72">
+        <v>13.4602</v>
+      </c>
+      <c r="M22" s="72">
+        <v>188.6278</v>
+      </c>
+      <c r="N22" s="72">
+        <v>33.3646</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="B23" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s" s="68">
+        <v>28</v>
+      </c>
+      <c r="D23" s="89">
+        <v>4</v>
+      </c>
+      <c r="E23" s="90">
+        <v>4</v>
+      </c>
+      <c r="F23" s="68">
+        <v>8</v>
+      </c>
+      <c r="G23" s="68">
+        <v>48.0354</v>
+      </c>
+      <c r="H23" s="68">
+        <v>1.2482</v>
+      </c>
+      <c r="I23" s="68">
+        <v>48.3788</v>
+      </c>
+      <c r="J23" s="68">
+        <v>0.1816</v>
+      </c>
+      <c r="K23" s="68">
+        <v>48.9651</v>
+      </c>
+      <c r="L23" s="68">
+        <v>3.5017</v>
+      </c>
+      <c r="M23" s="68">
+        <v>0</v>
+      </c>
+      <c r="N23" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1">
+      <c r="B24" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s" s="72">
+        <v>29</v>
+      </c>
+      <c r="D24" s="86">
+        <v>4</v>
+      </c>
+      <c r="E24" s="87">
+        <v>4</v>
+      </c>
+      <c r="F24" s="72">
+        <v>16</v>
+      </c>
+      <c r="G24" s="72">
+        <v>48.4958</v>
+      </c>
+      <c r="H24" s="72">
+        <v>0.4048</v>
+      </c>
+      <c r="I24" s="72">
+        <v>48.2571</v>
+      </c>
+      <c r="J24" s="72">
+        <v>0.2206</v>
+      </c>
+      <c r="K24" s="72">
+        <v>49.5562</v>
+      </c>
+      <c r="L24" s="72">
+        <v>4.1184</v>
+      </c>
+      <c r="M24" s="72">
+        <v>0</v>
+      </c>
+      <c r="N24" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" ht="20.15" customHeight="1">
+      <c r="B25" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s" s="68">
+        <v>30</v>
+      </c>
+      <c r="D25" s="89">
+        <v>7</v>
+      </c>
+      <c r="E25" s="90">
+        <v>8</v>
+      </c>
+      <c r="F25" s="68">
+        <v>8</v>
+      </c>
+      <c r="G25" s="68">
+        <v>96.917</v>
+      </c>
+      <c r="H25" s="69">
+        <v>1.0014</v>
+      </c>
+      <c r="I25" s="68">
+        <v>96.67149999999999</v>
+      </c>
+      <c r="J25" s="68">
+        <v>0.5256</v>
+      </c>
+      <c r="K25" s="68">
+        <v>96.1238</v>
+      </c>
+      <c r="L25" s="68">
+        <v>1.7942</v>
+      </c>
+      <c r="M25" s="68">
+        <v>0</v>
+      </c>
+      <c r="N25" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="20.35" customHeight="1">
+      <c r="B26" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s" s="72">
+        <v>31</v>
+      </c>
+      <c r="D26" s="86">
+        <v>4</v>
+      </c>
+      <c r="E26" s="87">
+        <v>8</v>
+      </c>
+      <c r="F26" s="72">
+        <v>8</v>
+      </c>
+      <c r="G26" s="72">
+        <v>97.3693</v>
+      </c>
+      <c r="H26" s="121">
+        <v>1.4487</v>
+      </c>
+      <c r="I26" s="72">
+        <v>96.7375</v>
+      </c>
+      <c r="J26" s="72">
+        <v>0.4937</v>
+      </c>
+      <c r="K26" s="72">
+        <v>95.9965</v>
+      </c>
+      <c r="L26" s="72">
+        <v>1.9912</v>
+      </c>
+      <c r="M26" s="72">
+        <v>0</v>
+      </c>
+      <c r="N26" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="20.15" customHeight="1">
+      <c r="B27" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s" s="68">
+        <v>32</v>
+      </c>
+      <c r="D27" s="89">
+        <v>1</v>
+      </c>
+      <c r="E27" s="90">
+        <v>8</v>
+      </c>
+      <c r="F27" s="68">
+        <v>16</v>
+      </c>
+      <c r="G27" s="68">
+        <v>96.4753</v>
+      </c>
+      <c r="H27" s="122">
+        <v>0.7539</v>
+      </c>
+      <c r="I27" s="68">
+        <v>97.1396</v>
+      </c>
+      <c r="J27" s="68">
+        <v>0.4863</v>
+      </c>
+      <c r="K27" s="68">
+        <v>96.64619999999999</v>
+      </c>
+      <c r="L27" s="68">
+        <v>2.4552</v>
+      </c>
+      <c r="M27" s="68">
+        <v>0</v>
+      </c>
+      <c r="N27" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1">
+      <c r="B28" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s" s="72">
+        <v>33</v>
+      </c>
+      <c r="D28" s="86">
+        <v>3</v>
+      </c>
+      <c r="E28" s="87">
+        <v>16</v>
+      </c>
+      <c r="F28" s="72">
+        <v>8</v>
+      </c>
+      <c r="G28" s="72">
+        <v>193.8624</v>
+      </c>
+      <c r="H28" s="72">
+        <v>8.0861</v>
+      </c>
+      <c r="I28" s="72">
+        <v>194.9085</v>
+      </c>
+      <c r="J28" s="72">
+        <v>4.2517</v>
+      </c>
+      <c r="K28" s="72">
+        <v>193.9645</v>
+      </c>
+      <c r="L28" s="72">
+        <v>24.2768</v>
+      </c>
+      <c r="M28" s="72">
+        <v>0</v>
+      </c>
+      <c r="N28" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="B29" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s" s="68">
+        <v>34</v>
+      </c>
+      <c r="D29" s="89">
+        <v>2</v>
+      </c>
+      <c r="E29" s="90">
+        <v>16</v>
+      </c>
+      <c r="F29" s="68">
+        <v>16</v>
+      </c>
+      <c r="G29" s="68">
+        <v>193.5828</v>
+      </c>
+      <c r="H29" s="68">
+        <v>5.0253</v>
+      </c>
+      <c r="I29" s="68">
+        <v>193.7174</v>
+      </c>
+      <c r="J29" s="68">
+        <v>2.3587</v>
+      </c>
+      <c r="K29" s="68">
+        <v>193.6413</v>
+      </c>
+      <c r="L29" s="68">
+        <v>8.586600000000001</v>
+      </c>
+      <c r="M29" s="68">
+        <v>0</v>
+      </c>
+      <c r="N29" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="B30" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s" s="72">
+        <v>35</v>
+      </c>
+      <c r="D30" s="86">
+        <v>22</v>
+      </c>
+      <c r="E30" s="87">
+        <v>16</v>
+      </c>
+      <c r="F30" s="72">
+        <v>16</v>
+      </c>
+      <c r="G30" s="72">
+        <v>194.441</v>
+      </c>
+      <c r="H30" s="72">
+        <v>4.6275</v>
+      </c>
+      <c r="I30" s="72">
+        <v>193.8906</v>
+      </c>
+      <c r="J30" s="72">
+        <v>2.1418</v>
+      </c>
+      <c r="K30" s="72">
+        <v>198.3383</v>
+      </c>
+      <c r="L30" s="72">
+        <v>8.837899999999999</v>
+      </c>
+      <c r="M30" s="72">
+        <v>0</v>
+      </c>
+      <c r="N30" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="20.15" customHeight="1">
+      <c r="B31" t="s" s="85">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s" s="68">
+        <v>18</v>
+      </c>
+      <c r="D31" s="89">
+        <v>16</v>
+      </c>
+      <c r="E31" s="90">
+        <v>8</v>
+      </c>
+      <c r="F31" s="68">
+        <v>8</v>
+      </c>
+      <c r="G31" s="68">
+        <v>94.86069999999999</v>
+      </c>
+      <c r="H31" s="68">
+        <v>1.4684</v>
+      </c>
+      <c r="I31" s="68">
+        <v>94.7311</v>
+      </c>
+      <c r="J31" s="68">
+        <v>1.9928</v>
+      </c>
+      <c r="K31" s="68">
+        <v>94.99469999999999</v>
+      </c>
+      <c r="L31" s="68">
+        <v>1.5695</v>
+      </c>
+      <c r="M31" s="89">
+        <v>95.3229</v>
+      </c>
+      <c r="N31" s="123">
+        <v>13.4943</v>
+      </c>
+    </row>
+    <row r="32" ht="20.35" customHeight="1">
+      <c r="B32" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s" s="72">
+        <v>19</v>
+      </c>
+      <c r="D32" s="86">
+        <v>2</v>
+      </c>
+      <c r="E32" s="87">
+        <v>8</v>
+      </c>
+      <c r="F32" s="72">
+        <v>8</v>
+      </c>
+      <c r="G32" s="72">
+        <v>94.02370000000001</v>
+      </c>
+      <c r="H32" s="72">
+        <v>1.8506</v>
+      </c>
+      <c r="I32" s="72">
+        <v>93.6187</v>
+      </c>
+      <c r="J32" s="72">
+        <v>2.3835</v>
+      </c>
+      <c r="K32" s="72">
+        <v>93.98309999999999</v>
+      </c>
+      <c r="L32" s="72">
+        <v>1.6944</v>
+      </c>
+      <c r="M32" s="86">
+        <v>92.26139999999999</v>
+      </c>
+      <c r="N32" s="29">
+        <v>11.1204</v>
+      </c>
+    </row>
+    <row r="33" ht="20.35" customHeight="1">
+      <c r="B33" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s" s="68">
+        <v>20</v>
+      </c>
+      <c r="D33" s="89">
+        <v>2</v>
+      </c>
+      <c r="E33" s="90">
+        <v>8</v>
+      </c>
+      <c r="F33" s="68">
+        <v>16</v>
+      </c>
+      <c r="G33" s="68">
+        <v>90.27290000000001</v>
+      </c>
+      <c r="H33" s="68">
+        <v>2.7171</v>
+      </c>
+      <c r="I33" s="68">
+        <v>93.0857</v>
+      </c>
+      <c r="J33" s="68">
+        <v>0.8032</v>
+      </c>
+      <c r="K33" s="68">
+        <v>92.4858</v>
+      </c>
+      <c r="L33" s="68">
+        <v>2.272</v>
+      </c>
+      <c r="M33" s="68">
+        <v>94.90049999999999</v>
+      </c>
+      <c r="N33" s="105">
+        <v>6.0652</v>
+      </c>
+    </row>
+    <row r="34" ht="20.35" customHeight="1">
+      <c r="B34" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="72">
+        <v>21</v>
+      </c>
+      <c r="D34" s="86">
+        <v>3</v>
+      </c>
+      <c r="E34" s="87">
+        <v>16</v>
+      </c>
+      <c r="F34" s="72">
+        <v>8</v>
+      </c>
+      <c r="G34" s="72">
+        <v>187.1908</v>
+      </c>
+      <c r="H34" s="72">
+        <v>10.1278</v>
+      </c>
+      <c r="I34" s="72">
+        <v>190.6449</v>
+      </c>
+      <c r="J34" s="72">
+        <v>23.5806</v>
+      </c>
+      <c r="K34" s="72">
+        <v>187.3632</v>
+      </c>
+      <c r="L34" s="72">
+        <v>22.7869</v>
+      </c>
+      <c r="M34" s="72">
+        <v>187.8501</v>
+      </c>
+      <c r="N34" s="104">
+        <v>53.6012</v>
+      </c>
+    </row>
+    <row r="35" ht="20.35" customHeight="1">
+      <c r="B35" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s" s="68">
+        <v>23</v>
+      </c>
+      <c r="D35" s="89">
+        <v>10</v>
+      </c>
+      <c r="E35" s="90">
+        <v>16</v>
+      </c>
+      <c r="F35" s="68">
+        <v>16</v>
+      </c>
+      <c r="G35" s="68">
+        <v>185.6508</v>
+      </c>
+      <c r="H35" s="68">
+        <v>6.4955</v>
+      </c>
+      <c r="I35" s="68">
+        <v>186.5406</v>
+      </c>
+      <c r="J35" s="68">
+        <v>12.8605</v>
+      </c>
+      <c r="K35" s="68">
+        <v>184.8077</v>
+      </c>
+      <c r="L35" s="68">
+        <v>9.020300000000001</v>
+      </c>
+      <c r="M35" s="68">
+        <v>208.9805</v>
+      </c>
+      <c r="N35" s="105">
+        <v>62.4933</v>
+      </c>
+    </row>
+    <row r="36" ht="20.35" customHeight="1">
+      <c r="B36" t="s" s="91">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s" s="72">
+        <v>24</v>
+      </c>
+      <c r="D36" s="86">
+        <v>2</v>
+      </c>
+      <c r="E36" s="87">
+        <v>16</v>
+      </c>
+      <c r="F36" s="72">
+        <v>16</v>
+      </c>
+      <c r="G36" s="72">
+        <v>184.1038</v>
+      </c>
+      <c r="H36" s="72">
+        <v>6.9355</v>
+      </c>
+      <c r="I36" s="72">
+        <v>188.7219</v>
+      </c>
+      <c r="J36" s="72">
+        <v>10.3075</v>
+      </c>
+      <c r="K36" s="72">
+        <v>186.3452</v>
+      </c>
+      <c r="L36" s="72">
+        <v>14.9657</v>
+      </c>
+      <c r="M36" s="86">
+        <v>194.1702</v>
+      </c>
+      <c r="N36" s="29">
+        <v>66.8869</v>
+      </c>
+    </row>
+    <row r="37" ht="20.15" customHeight="1">
+      <c r="B37" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s" s="68">
+        <v>28</v>
+      </c>
+      <c r="D37" s="89">
+        <v>3</v>
+      </c>
+      <c r="E37" s="90">
+        <v>4</v>
+      </c>
+      <c r="F37" s="68">
+        <v>8</v>
+      </c>
+      <c r="G37" s="68">
+        <v>48.0093</v>
+      </c>
+      <c r="H37" s="68">
+        <v>0.5485</v>
+      </c>
+      <c r="I37" s="68">
+        <v>48.1834</v>
+      </c>
+      <c r="J37" s="68">
+        <v>0.3826</v>
+      </c>
+      <c r="K37" s="68">
+        <v>48.3782</v>
+      </c>
+      <c r="L37" s="68">
+        <v>0.6291</v>
+      </c>
+      <c r="M37" s="89">
+        <v>0</v>
+      </c>
+      <c r="N37" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1">
+      <c r="B38" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s" s="72">
+        <v>29</v>
+      </c>
+      <c r="D38" s="86">
+        <v>2</v>
+      </c>
+      <c r="E38" s="87">
+        <v>4</v>
+      </c>
+      <c r="F38" s="72">
+        <v>16</v>
+      </c>
+      <c r="G38" s="72">
+        <v>47.9242</v>
+      </c>
+      <c r="H38" s="72">
+        <v>0.6165</v>
+      </c>
+      <c r="I38" s="72">
+        <v>48.4239</v>
+      </c>
+      <c r="J38" s="72">
+        <v>0.4343</v>
+      </c>
+      <c r="K38" s="72">
+        <v>48.6302</v>
+      </c>
+      <c r="L38" s="72">
+        <v>1.5909</v>
+      </c>
+      <c r="M38" s="72">
+        <v>0</v>
+      </c>
+      <c r="N38" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="20.15" customHeight="1">
+      <c r="B39" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s" s="68">
+        <v>30</v>
+      </c>
+      <c r="D39" s="89">
+        <v>19</v>
+      </c>
+      <c r="E39" s="90">
+        <v>8</v>
+      </c>
+      <c r="F39" s="68">
+        <v>8</v>
+      </c>
+      <c r="G39" s="68">
+        <v>95.9987</v>
+      </c>
+      <c r="H39" s="69">
+        <v>0.7318</v>
+      </c>
+      <c r="I39" s="68">
+        <v>95.3258</v>
+      </c>
+      <c r="J39" s="68">
+        <v>1.3285</v>
+      </c>
+      <c r="K39" s="68">
+        <v>96.83629999999999</v>
+      </c>
+      <c r="L39" s="68">
+        <v>1.4306</v>
+      </c>
+      <c r="M39" s="68">
+        <v>0</v>
+      </c>
+      <c r="N39" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="20.35" customHeight="1">
+      <c r="B40" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s" s="72">
+        <v>31</v>
+      </c>
+      <c r="D40" s="86">
+        <v>1</v>
+      </c>
+      <c r="E40" s="87">
+        <v>8</v>
+      </c>
+      <c r="F40" s="72">
+        <v>8</v>
+      </c>
+      <c r="G40" s="72">
+        <v>95.9071</v>
+      </c>
+      <c r="H40" s="121">
+        <v>0.9401</v>
+      </c>
+      <c r="I40" s="72">
+        <v>95.7604</v>
+      </c>
+      <c r="J40" s="72">
+        <v>1.499</v>
+      </c>
+      <c r="K40" s="72">
+        <v>97.0385</v>
+      </c>
+      <c r="L40" s="72">
+        <v>2.2269</v>
+      </c>
+      <c r="M40" s="72">
+        <v>0</v>
+      </c>
+      <c r="N40" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="20.15" customHeight="1">
+      <c r="B41" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s" s="68">
+        <v>32</v>
+      </c>
+      <c r="D41" s="89">
+        <v>4</v>
+      </c>
+      <c r="E41" s="90">
+        <v>8</v>
+      </c>
+      <c r="F41" s="68">
+        <v>16</v>
+      </c>
+      <c r="G41" s="68">
+        <v>95.60129999999999</v>
+      </c>
+      <c r="H41" s="122">
+        <v>1.03</v>
+      </c>
+      <c r="I41" s="68">
+        <v>95.8385</v>
+      </c>
+      <c r="J41" s="68">
+        <v>0.9679</v>
+      </c>
+      <c r="K41" s="68">
+        <v>96.7641</v>
+      </c>
+      <c r="L41" s="68">
+        <v>1.8774</v>
+      </c>
+      <c r="M41" s="68">
+        <v>0</v>
+      </c>
+      <c r="N41" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="B42" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s" s="72">
+        <v>33</v>
+      </c>
+      <c r="D42" s="86">
+        <v>2</v>
+      </c>
+      <c r="E42" s="87">
+        <v>16</v>
+      </c>
+      <c r="F42" s="72">
+        <v>8</v>
+      </c>
+      <c r="G42" s="72">
+        <v>191.5647</v>
+      </c>
+      <c r="H42" s="72">
+        <v>5.3579</v>
+      </c>
+      <c r="I42" s="72">
+        <v>192.1096</v>
+      </c>
+      <c r="J42" s="72">
+        <v>23.3616</v>
+      </c>
+      <c r="K42" s="72">
+        <v>188.3977</v>
+      </c>
+      <c r="L42" s="72">
+        <v>23.9724</v>
+      </c>
+      <c r="M42" s="72">
+        <v>0</v>
+      </c>
+      <c r="N42" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="B43" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s" s="68">
+        <v>34</v>
+      </c>
+      <c r="D43" s="89">
+        <v>3</v>
+      </c>
+      <c r="E43" s="90">
+        <v>16</v>
+      </c>
+      <c r="F43" s="68">
+        <v>16</v>
+      </c>
+      <c r="G43" s="68">
+        <v>190.4741</v>
+      </c>
+      <c r="H43" s="68">
+        <v>3.9648</v>
+      </c>
+      <c r="I43" s="68">
+        <v>189.8284</v>
+      </c>
+      <c r="J43" s="68">
+        <v>6.7575</v>
+      </c>
+      <c r="K43" s="68">
+        <v>194.3592</v>
+      </c>
+      <c r="L43" s="68">
+        <v>8.8499</v>
+      </c>
+      <c r="M43" s="68">
+        <v>0</v>
+      </c>
+      <c r="N43" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" ht="20.15" customHeight="1">
+      <c r="B44" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s" s="72">
+        <v>35</v>
+      </c>
+      <c r="D44" s="86">
+        <v>17</v>
+      </c>
+      <c r="E44" s="87">
+        <v>16</v>
+      </c>
+      <c r="F44" s="72">
+        <v>16</v>
+      </c>
+      <c r="G44" s="72">
+        <v>191.0115</v>
+      </c>
+      <c r="H44" s="72">
+        <v>3.4113</v>
+      </c>
+      <c r="I44" s="72">
+        <v>188.5061</v>
+      </c>
+      <c r="J44" s="72">
+        <v>6.3803</v>
+      </c>
+      <c r="K44" s="72">
+        <v>194.4348</v>
+      </c>
+      <c r="L44" s="72">
+        <v>8.8903</v>
+      </c>
+      <c r="M44" s="72">
+        <v>0</v>
+      </c>
+      <c r="N44" s="124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" ht="20.35" customHeight="1">
+      <c r="B45" t="s" s="85">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s" s="68">
+        <v>18</v>
+      </c>
+      <c r="D45" s="89">
+        <v>5</v>
+      </c>
+      <c r="E45" s="90">
+        <v>8</v>
+      </c>
+      <c r="F45" s="68">
+        <v>8</v>
+      </c>
+      <c r="G45" s="68">
+        <v>93.7029</v>
+      </c>
+      <c r="H45" s="68">
+        <v>3.385</v>
+      </c>
+      <c r="I45" s="68">
+        <v>94.81359999999999</v>
+      </c>
+      <c r="J45" s="68">
+        <v>0.6999</v>
+      </c>
+      <c r="K45" s="68">
+        <v>95.1391</v>
+      </c>
+      <c r="L45" s="68">
+        <v>1.9639</v>
+      </c>
+      <c r="M45" s="89">
+        <v>98.1572</v>
+      </c>
+      <c r="N45" s="16">
+        <v>15.6852</v>
+      </c>
+    </row>
+    <row r="46" ht="20.35" customHeight="1">
+      <c r="B46" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s" s="72">
+        <v>19</v>
+      </c>
+      <c r="D46" s="86">
+        <v>1</v>
+      </c>
+      <c r="E46" s="87">
+        <v>8</v>
+      </c>
+      <c r="F46" s="72">
+        <v>8</v>
+      </c>
+      <c r="G46" s="72">
+        <v>93.0909</v>
+      </c>
+      <c r="H46" s="72">
+        <v>3.8252</v>
+      </c>
+      <c r="I46" s="72">
+        <v>94.16670000000001</v>
+      </c>
+      <c r="J46" s="72">
+        <v>0.8389</v>
+      </c>
+      <c r="K46" s="124">
+        <v>94.0491</v>
+      </c>
+      <c r="L46" s="125">
+        <v>2.044</v>
+      </c>
+      <c r="M46" s="86">
+        <v>97.79989999999999</v>
+      </c>
+      <c r="N46" s="29">
+        <v>12.9781</v>
+      </c>
+    </row>
+    <row r="47" ht="20.35" customHeight="1">
+      <c r="B47" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s" s="68">
+        <v>20</v>
+      </c>
+      <c r="D47" s="89">
+        <v>3</v>
+      </c>
+      <c r="E47" s="90">
+        <v>8</v>
+      </c>
+      <c r="F47" s="68">
+        <v>16</v>
+      </c>
+      <c r="G47" s="68">
+        <v>90.27290000000001</v>
+      </c>
+      <c r="H47" s="68">
+        <v>2.7171</v>
+      </c>
+      <c r="I47" s="68">
+        <v>93.0857</v>
+      </c>
+      <c r="J47" s="68">
+        <v>0.8032</v>
+      </c>
+      <c r="K47" s="105">
+        <v>92.4858</v>
+      </c>
+      <c r="L47" s="88">
+        <v>2.272</v>
+      </c>
+      <c r="M47" s="68">
+        <v>94.90049999999999</v>
+      </c>
+      <c r="N47" s="105">
+        <v>6.0652</v>
+      </c>
+    </row>
+    <row r="48" ht="20.35" customHeight="1">
+      <c r="B48" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s" s="72">
+        <v>21</v>
+      </c>
+      <c r="D48" s="86">
+        <v>2</v>
+      </c>
+      <c r="E48" s="87">
+        <v>16</v>
+      </c>
+      <c r="F48" s="72">
+        <v>8</v>
+      </c>
+      <c r="G48" s="72">
+        <v>188.469</v>
+      </c>
+      <c r="H48" s="72">
+        <v>20.4162</v>
+      </c>
+      <c r="I48" s="72">
+        <v>189.2267</v>
+      </c>
+      <c r="J48" s="72">
+        <v>8.4526</v>
+      </c>
+      <c r="K48" s="104">
+        <v>187.213</v>
+      </c>
+      <c r="L48" s="112">
+        <v>22.7381</v>
+      </c>
+      <c r="M48" s="72">
+        <v>198.6514</v>
+      </c>
+      <c r="N48" s="104">
+        <v>51.675</v>
+      </c>
+    </row>
+    <row r="49" ht="20.35" customHeight="1">
+      <c r="B49" t="s" s="88">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s" s="68">
+        <v>23</v>
+      </c>
+      <c r="D49" s="89">
+        <v>7</v>
+      </c>
+      <c r="E49" s="90">
+        <v>16</v>
+      </c>
+      <c r="F49" s="68">
+        <v>16</v>
+      </c>
+      <c r="G49" s="68">
+        <v>187.6019</v>
+      </c>
+      <c r="H49" s="68">
+        <v>11.2079</v>
+      </c>
+      <c r="I49" s="68">
+        <v>187.5061</v>
+      </c>
+      <c r="J49" s="68">
+        <v>4.7104</v>
+      </c>
+      <c r="K49" s="105">
+        <v>188.3484</v>
+      </c>
+      <c r="L49" s="88">
+        <v>10.7142</v>
+      </c>
+      <c r="M49" s="68">
+        <v>191.2378</v>
+      </c>
+      <c r="N49" s="105">
+        <v>36.6428</v>
+      </c>
+    </row>
+    <row r="50" ht="20.35" customHeight="1">
+      <c r="B50" t="s" s="91">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s" s="72">
+        <v>24</v>
+      </c>
+      <c r="D50" s="86">
+        <v>3</v>
+      </c>
+      <c r="E50" s="87">
+        <v>16</v>
+      </c>
+      <c r="F50" s="72">
+        <v>16</v>
+      </c>
+      <c r="G50" s="72">
+        <v>185.3288</v>
+      </c>
+      <c r="H50" s="72">
+        <v>13.9402</v>
+      </c>
+      <c r="I50" s="72">
+        <v>187.1187</v>
+      </c>
+      <c r="J50" s="72">
+        <v>4.5497</v>
+      </c>
+      <c r="K50" s="104">
+        <v>190.0643</v>
+      </c>
+      <c r="L50" s="29">
+        <v>16.7014</v>
+      </c>
+      <c r="M50" s="126">
+        <v>173.6851</v>
+      </c>
+      <c r="N50" s="106">
+        <v>32.7498</v>
+      </c>
+    </row>
+    <row r="51" ht="20.35" customHeight="1">
+      <c r="B51" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s" s="68">
+        <v>28</v>
+      </c>
+      <c r="D51" s="89">
+        <v>1</v>
+      </c>
+      <c r="E51" s="90">
+        <v>4</v>
+      </c>
+      <c r="F51" s="68">
+        <v>8</v>
+      </c>
+      <c r="G51" s="68">
+        <v>48.1388</v>
+      </c>
+      <c r="H51" s="68">
+        <v>0.5865</v>
+      </c>
+      <c r="I51" s="68">
+        <v>48.1169</v>
+      </c>
+      <c r="J51" s="68">
+        <v>0.1886</v>
+      </c>
+      <c r="K51" s="105">
+        <v>48.242</v>
+      </c>
+      <c r="L51" s="88">
+        <v>0.7454</v>
+      </c>
+      <c r="M51" s="68">
+        <v>0</v>
+      </c>
+      <c r="N51" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" ht="20.35" customHeight="1">
+      <c r="B52" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s" s="72">
+        <v>29</v>
+      </c>
+      <c r="D52" s="86">
+        <v>3</v>
+      </c>
+      <c r="E52" s="87">
+        <v>4</v>
+      </c>
+      <c r="F52" s="72">
+        <v>16</v>
+      </c>
+      <c r="G52" s="72">
+        <v>47.6074</v>
+      </c>
+      <c r="H52" s="72">
+        <v>0.4337</v>
+      </c>
+      <c r="I52" s="72">
+        <v>48.3481</v>
+      </c>
+      <c r="J52" s="72">
+        <v>0.2361</v>
+      </c>
+      <c r="K52" s="104">
+        <v>47.9567</v>
+      </c>
+      <c r="L52" s="112">
+        <v>1.3286</v>
+      </c>
+      <c r="M52" s="72">
+        <v>0</v>
+      </c>
+      <c r="N52" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" ht="20.35" customHeight="1">
+      <c r="B53" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s" s="68">
+        <v>30</v>
+      </c>
+      <c r="D53" s="89">
+        <v>17</v>
+      </c>
+      <c r="E53" s="90">
+        <v>8</v>
+      </c>
+      <c r="F53" s="68">
+        <v>8</v>
+      </c>
+      <c r="G53" s="68">
+        <v>95.26990000000001</v>
+      </c>
+      <c r="H53" s="69">
+        <v>1.0294</v>
+      </c>
+      <c r="I53" s="68">
+        <v>94.6568</v>
+      </c>
+      <c r="J53" s="68">
+        <v>1.2803</v>
+      </c>
+      <c r="K53" s="105">
+        <v>96.3501</v>
+      </c>
+      <c r="L53" s="88">
+        <v>1.9308</v>
+      </c>
+      <c r="M53" s="68">
+        <v>0</v>
+      </c>
+      <c r="N53" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" ht="20.35" customHeight="1">
+      <c r="B54" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s" s="72">
+        <v>31</v>
+      </c>
+      <c r="D54" s="86">
+        <v>2</v>
+      </c>
+      <c r="E54" s="87">
+        <v>8</v>
+      </c>
+      <c r="F54" s="72">
+        <v>8</v>
+      </c>
+      <c r="G54" s="72">
+        <v>95.4485</v>
+      </c>
+      <c r="H54" s="121">
+        <v>1.1108</v>
+      </c>
+      <c r="I54" s="72">
+        <v>94.6802</v>
+      </c>
+      <c r="J54" s="72">
+        <v>1.0343</v>
+      </c>
+      <c r="K54" s="104">
+        <v>96.01730000000001</v>
+      </c>
+      <c r="L54" s="112">
+        <v>1.6618</v>
+      </c>
+      <c r="M54" s="72">
+        <v>0</v>
+      </c>
+      <c r="N54" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" ht="20.35" customHeight="1">
+      <c r="B55" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C55" t="s" s="68">
+        <v>32</v>
+      </c>
+      <c r="D55" s="89">
+        <v>2</v>
+      </c>
+      <c r="E55" s="90">
+        <v>8</v>
+      </c>
+      <c r="F55" s="68">
+        <v>16</v>
+      </c>
+      <c r="G55" s="68">
+        <v>95.2436</v>
+      </c>
+      <c r="H55" s="122">
+        <v>0.9315</v>
+      </c>
+      <c r="I55" s="68">
+        <v>96.0347</v>
+      </c>
+      <c r="J55" s="68">
+        <v>0.5052</v>
+      </c>
+      <c r="K55" s="105">
+        <v>95.93899999999999</v>
+      </c>
+      <c r="L55" s="88">
+        <v>2.0378</v>
+      </c>
+      <c r="M55" s="68">
+        <v>0</v>
+      </c>
+      <c r="N55" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" ht="20.35" customHeight="1">
+      <c r="B56" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s" s="72">
+        <v>33</v>
+      </c>
+      <c r="D56" s="86">
+        <v>4</v>
+      </c>
+      <c r="E56" s="87">
+        <v>16</v>
+      </c>
+      <c r="F56" s="72">
+        <v>8</v>
+      </c>
+      <c r="G56" s="72">
+        <v>189.0281</v>
+      </c>
+      <c r="H56" s="72">
+        <v>6.375</v>
+      </c>
+      <c r="I56" s="72">
+        <v>188.7123</v>
+      </c>
+      <c r="J56" s="72">
+        <v>3.9701</v>
+      </c>
+      <c r="K56" s="104">
+        <v>199.5215</v>
+      </c>
+      <c r="L56" s="112">
+        <v>16.6594</v>
+      </c>
+      <c r="M56" s="72">
+        <v>0</v>
+      </c>
+      <c r="N56" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" ht="20.35" customHeight="1">
+      <c r="B57" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s" s="68">
+        <v>34</v>
+      </c>
+      <c r="D57" s="89">
+        <v>1</v>
+      </c>
+      <c r="E57" s="90">
+        <v>16</v>
+      </c>
+      <c r="F57" s="68">
+        <v>16</v>
+      </c>
+      <c r="G57" s="68">
+        <v>188.8079</v>
+      </c>
+      <c r="H57" s="68">
+        <v>5.5961</v>
+      </c>
+      <c r="I57" s="68">
+        <v>190.4295</v>
+      </c>
+      <c r="J57" s="68">
+        <v>8.3233</v>
+      </c>
+      <c r="K57" s="105">
+        <v>187.4636</v>
+      </c>
+      <c r="L57" s="88">
+        <v>9.6448</v>
+      </c>
+      <c r="M57" s="68">
+        <v>0</v>
+      </c>
+      <c r="N57" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" ht="20.35" customHeight="1">
+      <c r="B58" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="C58" t="s" s="72">
+        <v>35</v>
+      </c>
+      <c r="D58" s="86">
+        <v>2</v>
+      </c>
+      <c r="E58" s="87">
+        <v>16</v>
+      </c>
+      <c r="F58" s="72">
+        <v>16</v>
+      </c>
+      <c r="G58" s="72">
+        <v>189.1698</v>
+      </c>
+      <c r="H58" s="72">
+        <v>5.1273</v>
+      </c>
+      <c r="I58" s="72">
+        <v>188.8348</v>
+      </c>
+      <c r="J58" s="72">
+        <v>8.140499999999999</v>
+      </c>
+      <c r="K58" s="104">
+        <v>189.6262</v>
+      </c>
+      <c r="L58" s="112">
+        <v>8.7575</v>
+      </c>
+      <c r="M58" s="72">
+        <v>0</v>
+      </c>
+      <c r="N58" s="72">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>